<commit_message>
data as requested on slack - see extra excel sheets
</commit_message>
<xml_diff>
--- a/ComparingScenarios.xlsx
+++ b/ComparingScenarios.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pfeiffa/Documents/GitHub/Suiattle_NST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C03565E-4325-0D42-A286-1E60235F9272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EEF48DB-21BF-A044-B69A-AF2EF066D6C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1500" yWindow="1320" windowWidth="27640" windowHeight="16940" xr2:uid="{12D1168B-7926-EF4B-BABE-130ECEEFFA7C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4924" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4936" uniqueCount="8">
   <si>
     <t>percent_added_pulse</t>
   </si>
@@ -52,17 +55,39 @@
   <si>
     <t>nan</t>
   </si>
+  <si>
+    <t>Number of pulse parcels that left the network</t>
+  </si>
+  <si>
+    <t>max vol pulse abraded</t>
+  </si>
+  <si>
+    <t>vol pulse left network (max)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF1D1C1D"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -86,8 +111,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F6D1512-9980-F043-B970-B7DE677279B6}">
   <dimension ref="A1:C2002"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1369" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -22449,4 +22476,130 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551A84C8-5D64-CA4D-9371-BFD861A6A09B}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>394</v>
+      </c>
+      <c r="C3">
+        <v>493</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2875F6DD-3C6C-6C43-8873-16C5883C9E14}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>425</v>
+      </c>
+      <c r="B3">
+        <v>7636.1207435111201</v>
+      </c>
+      <c r="C3">
+        <v>10750.1023720761</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C14DC9-0608-8048-9548-BC5566054F52}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>302726.638640397</v>
+      </c>
+      <c r="C3">
+        <v>561458.14217985398</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>